<commit_message>
test shopping cart added
</commit_message>
<xml_diff>
--- a/com.ebay/src/test/resources/test_data.xlsx
+++ b/com.ebay/src/test/resources/test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.ebay\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0CDD77-2CF2-4C2C-A7EB-481D7F57D6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3065C9-A14B-4B7A-9743-75182D1BB46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86415615-9FB9-46A9-B5C3-822528024EBF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{86415615-9FB9-46A9-B5C3-822528024EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="doSearch" sheetId="1" r:id="rId1"/>
+    <sheet name="doSignIn" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Search Term</t>
   </si>
@@ -49,19 +50,56 @@
   </si>
   <si>
     <t xml:space="preserve">Freezer Bags </t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password </t>
+  </si>
+  <si>
+    <t>justin.smith1@gmail.com</t>
+  </si>
+  <si>
+    <t>AydenLiam1213@</t>
+  </si>
+  <si>
+    <t>goodbook926@gmail.com</t>
+  </si>
+  <si>
+    <t>Auooz Akbar1996</t>
+  </si>
+  <si>
+    <t>anoor37290@gmail.com</t>
+  </si>
+  <si>
+    <t>Serpent9999+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF202124"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,13 +119,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -402,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE62EC40-3A32-4E58-A7E9-5F47DFE95EAD}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -439,4 +481,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F61DA2-F7E0-4F50-8D85-7D82629EC273}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{3C755434-45D7-4132-B95E-9B93F673DF31}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{13ACCF25-5FEA-4216-AE9F-D4DFA609433C}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{2A37AD5A-8D53-4B62-934C-E93E392B336A}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{9298421C-5DF0-492A-819E-B6FC4869FB84}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>